<commit_message>
edited rf, updated opcode
</commit_message>
<xml_diff>
--- a/opcode.xlsx
+++ b/opcode.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\200Project2\32bit_risc_cpu\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28698" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>OPC</t>
   </si>
@@ -158,19 +163,19 @@
   </si>
   <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>ADDF</t>
+  </si>
+  <si>
+    <t>MULF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,346 +183,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -525,251 +200,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -787,61 +220,17 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1099,22 +488,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.57142857142857" customWidth="1"/>
-    <col min="2" max="7" width="3.57142857142857" customWidth="1"/>
+    <col min="1" max="1" width="7.578125" customWidth="1"/>
+    <col min="2" max="7" width="3.578125" customWidth="1"/>
     <col min="8" max="8" width="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1174,11 +563,21 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -1190,10 +589,18 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
@@ -1208,10 +615,18 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
@@ -1226,9 +641,15 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
@@ -1246,9 +667,15 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
@@ -1266,9 +693,15 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
@@ -1286,9 +719,15 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
@@ -1306,8 +745,12 @@
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
@@ -1328,8 +771,12 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -1350,8 +797,12 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
@@ -1372,8 +823,12 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
@@ -1394,8 +849,12 @@
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
@@ -1416,8 +875,12 @@
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
@@ -1438,8 +901,12 @@
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
@@ -1460,8 +927,12 @@
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
@@ -1482,7 +953,9 @@
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18">
+        <v>0</v>
+      </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
@@ -1506,7 +979,9 @@
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19">
+        <v>0</v>
+      </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
@@ -1530,7 +1005,9 @@
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20">
+        <v>0</v>
+      </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
@@ -1554,7 +1031,9 @@
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21">
+        <v>0</v>
+      </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
@@ -1578,7 +1057,9 @@
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22">
+        <v>0</v>
+      </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
@@ -1602,7 +1083,9 @@
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23">
+        <v>0</v>
+      </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
@@ -1626,7 +1109,9 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24">
+        <v>0</v>
+      </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
@@ -1646,8 +1131,59 @@
         <v>47</v>
       </c>
     </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>